<commit_message>
Fix default purity for Deuterium, added D and N tests
</commit_message>
<xml_diff>
--- a/inst/extdata/N_Sample_Input_Simple.xlsx
+++ b/inst/extdata/N_Sample_Input_Simple.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="75">
   <si>
     <t xml:space="preserve">Compound</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t xml:space="preserve">N-acetyl-glutamate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C7H11NO5</t>
   </si>
   <si>
     <t xml:space="preserve">glutathione disulfide</t>
@@ -353,7 +356,7 @@
   <dimension ref="A1:W1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="B47" activeCellId="0" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3564,7 +3567,7 @@
         <v>47</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>25</v>
@@ -3635,7 +3638,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C47" s="0" t="s">
         <v>26</v>
@@ -3703,10 +3706,10 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>25</v>
@@ -3774,10 +3777,10 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>26</v>
@@ -3845,10 +3848,10 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>27</v>
@@ -3916,10 +3919,10 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C51" s="0" t="s">
         <v>28</v>
@@ -3987,10 +3990,10 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C52" s="0" t="s">
         <v>29</v>
@@ -4058,10 +4061,10 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>30</v>
@@ -4129,10 +4132,10 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C54" s="0" t="s">
         <v>31</v>
@@ -4200,10 +4203,10 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C55" s="0" t="s">
         <v>25</v>
@@ -4271,10 +4274,10 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C56" s="0" t="s">
         <v>26</v>
@@ -4342,10 +4345,10 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C57" s="0" t="s">
         <v>27</v>
@@ -4413,10 +4416,10 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>28</v>
@@ -4484,10 +4487,10 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C59" s="0" t="s">
         <v>29</v>
@@ -4555,10 +4558,10 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C60" s="0" t="s">
         <v>30</v>
@@ -4626,10 +4629,10 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C61" s="0" t="s">
         <v>25</v>
@@ -4697,10 +4700,10 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C62" s="0" t="s">
         <v>26</v>
@@ -4768,10 +4771,10 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C63" s="0" t="s">
         <v>27</v>
@@ -4839,10 +4842,10 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C64" s="0" t="s">
         <v>28</v>
@@ -4910,10 +4913,10 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C65" s="0" t="s">
         <v>29</v>
@@ -4981,10 +4984,10 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C66" s="0" t="s">
         <v>30</v>
@@ -5052,10 +5055,10 @@
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C67" s="0" t="s">
         <v>31</v>
@@ -5123,10 +5126,10 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C68" s="0" t="s">
         <v>32</v>
@@ -5194,10 +5197,10 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C69" s="0" t="s">
         <v>25</v>
@@ -5265,10 +5268,10 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C70" s="0" t="s">
         <v>26</v>
@@ -5336,10 +5339,10 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C71" s="0" t="s">
         <v>27</v>
@@ -5407,10 +5410,10 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C72" s="0" t="s">
         <v>28</v>
@@ -5478,10 +5481,10 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C73" s="0" t="s">
         <v>29</v>
@@ -5549,10 +5552,10 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C74" s="0" t="s">
         <v>25</v>
@@ -5620,10 +5623,10 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C75" s="0" t="s">
         <v>26</v>
@@ -5691,10 +5694,10 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C76" s="0" t="s">
         <v>27</v>
@@ -5762,10 +5765,10 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C77" s="0" t="s">
         <v>28</v>
@@ -5833,10 +5836,10 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C78" s="0" t="s">
         <v>25</v>
@@ -5904,10 +5907,10 @@
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C79" s="0" t="s">
         <v>26</v>
@@ -5975,10 +5978,10 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C80" s="0" t="s">
         <v>25</v>
@@ -6046,10 +6049,10 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C81" s="0" t="s">
         <v>26</v>
@@ -6117,10 +6120,10 @@
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C82" s="0" t="s">
         <v>25</v>
@@ -6188,10 +6191,10 @@
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C83" s="0" t="s">
         <v>26</v>
@@ -6259,10 +6262,10 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C84" s="0" t="s">
         <v>25</v>
@@ -6330,10 +6333,10 @@
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C85" s="0" t="s">
         <v>26</v>
@@ -6401,10 +6404,10 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C86" s="0" t="s">
         <v>25</v>
@@ -6472,10 +6475,10 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C87" s="0" t="s">
         <v>26</v>
@@ -6543,10 +6546,10 @@
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C88" s="0" t="s">
         <v>25</v>
@@ -6614,10 +6617,10 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C89" s="0" t="s">
         <v>26</v>
@@ -6685,10 +6688,10 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C90" s="0" t="s">
         <v>25</v>
@@ -6756,10 +6759,10 @@
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C91" s="0" t="s">
         <v>26</v>
@@ -6827,10 +6830,10 @@
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C92" s="0" t="s">
         <v>27</v>
@@ -6898,10 +6901,10 @@
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C93" s="0" t="s">
         <v>25</v>
@@ -6969,10 +6972,10 @@
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C94" s="0" t="s">
         <v>26</v>
@@ -7040,10 +7043,10 @@
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C95" s="0" t="s">
         <v>27</v>

</xml_diff>